<commit_message>
Delete Batch Program changes
</commit_message>
<xml_diff>
--- a/Data Files/LMSAPIHackathon.xlsx
+++ b/Data Files/LMSAPIHackathon.xlsx
@@ -5,36 +5,53 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse-numpyninja\LMSRestAssuredAutomation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABCD194-8908-4168-A7D2-71468272342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9499DE9-CD32-487F-93D1-596CB03FC6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getsingleprogram" sheetId="1" r:id="rId1"/>
     <sheet name="getsingleprograminvalid" sheetId="2" r:id="rId2"/>
     <sheet name="getsingleprograminvalidinput" sheetId="3" r:id="rId3"/>
+    <sheet name="deleteProgram" sheetId="4" r:id="rId4"/>
+    <sheet name="deleteBatch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>programId</t>
   </si>
   <si>
     <t>**</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>"Jan23-NinjaCreators-SDET-00002"</t>
+  </si>
+  <si>
+    <t>Jan23-NinjaCreators12-SDET-00001</t>
+  </si>
+  <si>
+    <t>batchId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -52,6 +69,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -80,10 +110,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,7 +340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -329,7 +363,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -350,11 +384,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8AD398-E207-49CF-984E-7F93D9D4A840}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -369,4 +403,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583A17EC-F2BC-4BC0-AF56-98D23A8D8117}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1958</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BA8418-7EDB-453B-A206-AC6390AE3DAB}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>694</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified some of Delete and added logging
</commit_message>
<xml_diff>
--- a/Data Files/LMSAPIHackathon.xlsx
+++ b/Data Files/LMSAPIHackathon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\eclipse-workspace\LMSRestAssuredAutomation\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse-numpyninja\LMSRestAssuredAutomation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5462842-3E76-4C45-9D8F-27FB0D75EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F184D1FD-16DA-48AA-956B-6CC1EA984ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getsingleprogram" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,16 @@
     <sheet name="NoProgStaus" sheetId="7" r:id="rId5"/>
     <sheet name="NoProgDescription" sheetId="6" r:id="rId6"/>
     <sheet name="NoProgramName" sheetId="5" r:id="rId7"/>
+    <sheet name="deleteProgram" sheetId="8" r:id="rId8"/>
+    <sheet name="deleteBatch" sheetId="9" r:id="rId9"/>
+    <sheet name="postBatchValid" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>programId</t>
   </si>
@@ -83,13 +86,49 @@
   </si>
   <si>
     <t>Java J2EE</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>"Jan23-NinjaCreators-SDET-00002"</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Jan23-NinjaCreators12-SDET-00001</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>batchName</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>Jan23-NinjaCreators-SDETbatch-001</t>
+  </si>
+  <si>
+    <t>Jan23-NinjaCreators-SDETbatch-002</t>
+  </si>
+  <si>
+    <t>Jan23-NinjaCreators-SDETbatch-003</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -126,6 +165,18 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -150,18 +201,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4E605D4E-8E8B-436F-9991-8A1EFA4ECB9B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,7 +439,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -398,19 +456,83 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E468C129-7920-4F40-BA2E-0EEAC4AF4EB3}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C5D131-B538-4A7D-A90E-825DE99BF868}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,11 +593,11 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,15 +628,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B140CD73-F2E8-4D82-B9E9-D6F2037B6DDA}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,10 +687,10 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,10 +722,10 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,10 +757,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,4 +782,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E231B6A0-0E13-4B0D-90BE-D23F52E9B22B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1958</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25BCA2-37FA-4F40-BEE9-D29CC211C478}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correcting duplicate step def across Delete
</commit_message>
<xml_diff>
--- a/Data Files/LMSAPIHackathon.xlsx
+++ b/Data Files/LMSAPIHackathon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse-numpyninja\LMSRestAssuredAutomation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F184D1FD-16DA-48AA-956B-6CC1EA984ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD2854A-A74D-444B-9AA1-331BE5DF64B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
     <t>Jan23-NinjaCreators-SDETbatch-003</t>
   </si>
   <si>
-    <t>Inactive</t>
+    <t>Salesforce1</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -509,10 +509,10 @@
         <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing changes for BatchGet module
</commit_message>
<xml_diff>
--- a/Data Files/LMSAPIHackathon.xlsx
+++ b/Data Files/LMSAPIHackathon.xlsx
@@ -1,35 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse-numpyninja\LMSRestAssuredAutomation\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse\LMSRestAssuredAutomation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD2854A-A74D-444B-9AA1-331BE5DF64B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C5BA90-E11C-4427-9CCC-7F5E9F5EC59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getsingleprogram" sheetId="1" r:id="rId1"/>
-    <sheet name="postvaliddataprogram" sheetId="2" r:id="rId2"/>
-    <sheet name="postinvalidprogramdata" sheetId="3" r:id="rId3"/>
-    <sheet name="RequestBodyInvalidData" sheetId="4" r:id="rId4"/>
-    <sheet name="NoProgStaus" sheetId="7" r:id="rId5"/>
-    <sheet name="NoProgDescription" sheetId="6" r:id="rId6"/>
-    <sheet name="NoProgramName" sheetId="5" r:id="rId7"/>
-    <sheet name="deleteProgram" sheetId="8" r:id="rId8"/>
-    <sheet name="deleteBatch" sheetId="9" r:id="rId9"/>
-    <sheet name="postBatchValid" sheetId="10" r:id="rId10"/>
+    <sheet name="getsinglebatch" sheetId="11" r:id="rId2"/>
+    <sheet name="getsinglebatchinvalidid" sheetId="12" r:id="rId3"/>
+    <sheet name="getsinglebatchname" sheetId="13" r:id="rId4"/>
+    <sheet name="getinvalidbatchname" sheetId="14" r:id="rId5"/>
+    <sheet name="getinvalidbatchprogramid" sheetId="15" r:id="rId6"/>
+    <sheet name="postvaliddataprogram" sheetId="2" r:id="rId7"/>
+    <sheet name="postinvalidprogramdata" sheetId="3" r:id="rId8"/>
+    <sheet name="RequestBodyInvalidData" sheetId="4" r:id="rId9"/>
+    <sheet name="NoProgStaus" sheetId="7" r:id="rId10"/>
+    <sheet name="NoProgDescription" sheetId="6" r:id="rId11"/>
+    <sheet name="NoProgramName" sheetId="5" r:id="rId12"/>
+    <sheet name="deleteProgram" sheetId="8" r:id="rId13"/>
+    <sheet name="deleteBatch" sheetId="9" r:id="rId14"/>
+    <sheet name="postBatchValid" sheetId="10" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>programId</t>
   </si>
@@ -122,6 +127,9 @@
   </si>
   <si>
     <t>Salesforce1</t>
+  </si>
+  <si>
+    <t>456**</t>
   </si>
 </sst>
 </file>
@@ -205,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -214,6 +222,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -437,7 +448,9 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -457,10 +470,198 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F678EAA-19FE-4BB5-917D-2E034BA184CB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F842BC-2127-4547-B67E-73C1D888E653}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C92B08D-31C7-450B-AEC7-BB013C23A9AE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E231B6A0-0E13-4B0D-90BE-D23F52E9B22B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1958</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25BCA2-37FA-4F40-BEE9-D29CC211C478}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E468C129-7920-4F40-BA2E-0EEAC4AF4EB3}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -521,6 +722,133 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587EAFE3-EE3C-49AA-94BA-B3C70F17ECCE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F57874C-797C-4DFE-A9AA-FC22A78E1317}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635B90C1-B9D5-4CBA-915B-D855473D9FA0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA0615C-370F-4AB2-97D1-31F4FFBC10F1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5AEC2F-8392-449D-A744-AA86D7629CBD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C5D131-B538-4A7D-A90E-825DE99BF868}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -585,7 +913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC12467-6CBD-40A9-8A18-9DDFECAE6CB6}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -624,12 +952,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B140CD73-F2E8-4D82-B9E9-D6F2037B6DDA}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -677,192 +1005,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F678EAA-19FE-4BB5-917D-2E034BA184CB}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F842BC-2127-4547-B67E-73C1D888E653}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C92B08D-31C7-450B-AEC7-BB013C23A9AE}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E231B6A0-0E13-4B0D-90BE-D23F52E9B22B}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="2" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1958</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25BCA2-37FA-4F40-BEE9-D29CC211C478}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="8.88671875" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BatchPost, BatchPut, ProgramPut changes from Valli and Sapna
</commit_message>
<xml_diff>
--- a/Data Files/LMSAPIHackathon.xlsx
+++ b/Data Files/LMSAPIHackathon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse\LMSRestAssuredAutomation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C5BA90-E11C-4427-9CCC-7F5E9F5EC59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDD8967-EB7E-4612-BFD6-6EF64440CD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getsingleprogram" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,20 @@
     <sheet name="deleteProgram" sheetId="8" r:id="rId13"/>
     <sheet name="deleteBatch" sheetId="9" r:id="rId14"/>
     <sheet name="postBatchValid" sheetId="10" r:id="rId15"/>
+    <sheet name="PostValidDataBatch" sheetId="16" r:id="rId16"/>
+    <sheet name="NoBatchName" sheetId="17" r:id="rId17"/>
+    <sheet name="PostInvalidDataBatch" sheetId="18" r:id="rId18"/>
+    <sheet name="NoBatchDescription" sheetId="19" r:id="rId19"/>
+    <sheet name="NoBatchStatus" sheetId="20" r:id="rId20"/>
+    <sheet name="NoBatchClasses" sheetId="21" r:id="rId21"/>
+    <sheet name="NoProgramId" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="40">
   <si>
     <t>programId</t>
   </si>
@@ -130,13 +137,37 @@
   </si>
   <si>
     <t>456**</t>
+  </si>
+  <si>
+    <t>!@#$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server basics </t>
+  </si>
+  <si>
+    <t>SQL BootCamp527</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>batchNoOfClasses</t>
+  </si>
+  <si>
+    <t>!@#</t>
+  </si>
+  <si>
+    <t>"509"</t>
+  </si>
+  <si>
+    <t>SQL Bootcamp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -185,6 +216,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -209,11 +247,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -227,8 +266,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4E605D4E-8E8B-436F-9991-8A1EFA4ECB9B}"/>
   </cellStyles>
@@ -721,11 +762,441 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCD4143-38F7-4731-9CBD-CD3DFC7DB142}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>509</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>509</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{AAB6958B-7C31-4F15-A849-E4BEE678489B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19704147-BDB5-4EEB-8FD6-5891D0B832F4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2450AE-0F6F-4A65-9284-0CE37E74F51B}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>-3</v>
+      </c>
+      <c r="E9">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>-509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{467F7FD4-D32B-4409-AB35-F5B54AF592C3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1DEE12-C096-4B54-80F8-32288ED7E284}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587EAFE3-EE3C-49AA-94BA-B3C70F17ECCE}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -739,6 +1210,138 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB365D9-AEA7-4A9B-8394-3F211F6EA393}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E73AF7B-254F-423D-A74B-AE1C4174D3BD}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9003988-F73D-4EA2-825F-DEA8FDB4A73F}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>